<commit_message>
Casi terminado una parte
</commit_message>
<xml_diff>
--- a/media/archivos/formato.xlsx
+++ b/media/archivos/formato.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de nacimiento (dd-mm-aa)</t>
+    <t xml:space="preserve">Nombre (*obligatorio)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de nacimiento (dd-mm-aa) (*obligatorio)</t>
   </si>
   <si>
     <t xml:space="preserve">Numero Playera</t>
@@ -231,10 +231,10 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.53"/>
@@ -242,7 +242,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>